<commit_message>
David Complted Pert Chart
</commit_message>
<xml_diff>
--- a/Documentation/GantChart.xlsx
+++ b/Documentation/GantChart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryangoudie/Documents/BSc Computer Science/Group Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E6B5ADA-D043-284E-8D5C-49309987BF5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADBC4B7-10C8-453D-AC24-E8BEC25F3498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1640" windowWidth="28040" windowHeight="17440" xr2:uid="{435CA23D-61D2-7248-B3A7-AE49617E1887}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{435CA23D-61D2-7248-B3A7-AE49617E1887}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>TimeLine</t>
   </si>
@@ -88,13 +87,52 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>PERT CHART DATA</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>PERT FORMULA</t>
+  </si>
+  <si>
+    <t>(O + (4*M) + P) / 6</t>
+  </si>
+  <si>
+    <t>Optimistic time(O)</t>
+  </si>
+  <si>
+    <t>Pessemistic Time(P)</t>
+  </si>
+  <si>
+    <t>Most Likely Time(M)</t>
+  </si>
+  <si>
+    <t>1.66…</t>
+  </si>
+  <si>
+    <t>EXPECTED INT</t>
+  </si>
+  <si>
+    <t>7.16…</t>
+  </si>
+  <si>
+    <t>9.16…</t>
+  </si>
+  <si>
+    <t>1.16…</t>
+  </si>
+  <si>
+    <t>3.833..</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,6 +152,22 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF424242"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,11 +190,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,7 +221,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -285,7 +345,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>44230</c:v>
@@ -1518,21 +1578,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CEF1AC1-7987-7240-8D4A-2E8AC0691667}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1617,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1566,7 +1628,7 @@
         <v>44232</v>
       </c>
       <c r="D2" s="1">
-        <f>C2-B2</f>
+        <f t="shared" ref="D2:D15" si="0">C2-B2</f>
         <v>2</v>
       </c>
       <c r="E2" s="1"/>
@@ -1579,7 +1641,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="21">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1590,7 +1652,7 @@
         <v>44232</v>
       </c>
       <c r="D3" s="1">
-        <f>C3-B3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E3" s="1"/>
@@ -1603,7 +1665,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="21">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1676,7 @@
         <v>44239</v>
       </c>
       <c r="D4" s="1">
-        <f>C4-B4</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E4" s="1"/>
@@ -1627,7 +1689,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="21">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1638,7 +1700,7 @@
         <v>44249</v>
       </c>
       <c r="D5" s="1">
-        <f>C5-B5</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E5" s="1"/>
@@ -1651,7 +1713,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="21">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1724,7 @@
         <v>44251</v>
       </c>
       <c r="D6" s="1">
-        <f>C6-B6</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E6" s="1"/>
@@ -1675,7 +1737,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="21">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1686,7 +1748,7 @@
         <v>44253</v>
       </c>
       <c r="D7" s="1">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E7" s="1"/>
@@ -1699,7 +1761,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="21">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1772,7 @@
         <v>44259</v>
       </c>
       <c r="D8" s="1">
-        <f>C8-B8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E8" s="1"/>
@@ -1723,7 +1785,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="21">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1734,7 +1796,7 @@
         <v>44265</v>
       </c>
       <c r="D9" s="1">
-        <f>C9-B9</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
@@ -1747,7 +1809,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="21">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1820,7 @@
         <v>44267</v>
       </c>
       <c r="D10" s="1">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" s="1"/>
@@ -1771,7 +1833,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="21">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1782,7 +1844,7 @@
         <v>44274</v>
       </c>
       <c r="D11" s="1">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E11" s="1"/>
@@ -1795,7 +1857,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="21">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1806,7 +1868,7 @@
         <v>44281</v>
       </c>
       <c r="D12" s="1">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E12" s="1"/>
@@ -1819,7 +1881,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="21">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1892,7 @@
         <v>44286</v>
       </c>
       <c r="D13" s="1">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E13" s="1"/>
@@ -1843,7 +1905,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="21">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1854,7 +1916,7 @@
         <v>44291</v>
       </c>
       <c r="D14" s="1">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E14" s="1"/>
@@ -1867,7 +1929,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="21">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1940,7 @@
         <v>44296</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E15" s="1"/>
@@ -1891,7 +1953,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="21">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1906,11 +1968,319 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="21">
       <c r="A17" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="21">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:9" ht="21">
+      <c r="A27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="21">
+      <c r="A28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="21">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>9</v>
+      </c>
+      <c r="D29" s="5">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="21">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30" s="5">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>13</v>
+      </c>
+      <c r="D31" s="5">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="21">
+      <c r="A32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" s="5">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="21">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="21">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="21">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="21">
+      <c r="A36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" s="5">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="21">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="21">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="21">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>